<commit_message>
Delete Student - Developing the Servlet and JDBC Code
</commit_message>
<xml_diff>
--- a/me_docs/13.Delete-Student.xlsx
+++ b/me_docs/13.Delete-Student.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E380F4-E2C3-40C4-81CA-ED655E63B63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AB8FA1-3C87-4383-837A-A86039026778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picture" sheetId="2" r:id="rId1"/>
     <sheet name="Creating the Delete Link" sheetId="1" r:id="rId2"/>
+    <sheet name="Creating the JDBC Code" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Add delete link in list-students.jsp</t>
   </si>
@@ -38,6 +39,27 @@
   </si>
   <si>
     <t>Click Delete</t>
+  </si>
+  <si>
+    <t>Create DeleteStudentControllerServlet</t>
+  </si>
+  <si>
+    <t>Init</t>
+  </si>
+  <si>
+    <t>doGet method</t>
+  </si>
+  <si>
+    <t>deleteStudent method in StudentDbUtil Class</t>
+  </si>
+  <si>
+    <t>Reset Server</t>
+  </si>
+  <si>
+    <t>Access URL to test</t>
+  </si>
+  <si>
+    <t>Data deleted</t>
   </si>
 </sst>
 </file>
@@ -311,6 +333,671 @@
         <a:xfrm>
           <a:off x="609600" y="16764000"/>
           <a:ext cx="9314286" cy="3676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>227733</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>170809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB288E5D-6897-442D-AD93-EFA91DB240BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6933333" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>570895</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E440A0-A975-45E4-B41A-0BCB576728A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="4838095" cy="3590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DDD248-BF64-4CD7-A54E-1107AA673FA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9525000"/>
+          <a:ext cx="4876190" cy="4638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>75619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC4D1201-E628-4057-BF46-A4BEF32A51D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14287500"/>
+          <a:ext cx="4866667" cy="4647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>560533</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>85095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FFDE58-E4D9-41F3-8EA6-DA73D49C6DC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19240500"/>
+          <a:ext cx="11533333" cy="5038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>169205</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F16DAC-AC69-4BCF-9B41-7413DDD04F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24384001"/>
+          <a:ext cx="11191875" cy="4931704"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>93790</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>27786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91432A0F-4222-406C-9706-DBA512FC6FBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="29527500"/>
+          <a:ext cx="11676190" cy="6314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8076</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>85095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8217631E-137D-485B-BE0C-1EAE5871715A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="36195000"/>
+          <a:ext cx="11590476" cy="5038095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>65219</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>113667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED03D3D3-BC74-49DC-BE3E-4A8D4EA93A42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="41529000"/>
+          <a:ext cx="11647619" cy="5066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>247</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>141333</xdr:colOff>
+      <xdr:row>273</xdr:row>
+      <xdr:rowOff>113667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46BB0CDA-E1CD-4ED1-8206-B6FA6A418353}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47053500"/>
+          <a:ext cx="12333333" cy="5066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>475200</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>27881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F11C68EC-FC32-43B9-ABBD-C8A2141F80F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52387500"/>
+          <a:ext cx="8400000" cy="5552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247009</xdr:colOff>
+      <xdr:row>330</xdr:row>
+      <xdr:rowOff>85167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB2A6C4-6586-4D66-BAFE-528CC3F8BF85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="58483500"/>
+          <a:ext cx="5123809" cy="4466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>332</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>179809</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>37643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EFB7A24-706F-44C6-9A35-9EF61E957026}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="63246000"/>
+          <a:ext cx="9323809" cy="3657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>371</xdr:row>
+      <xdr:rowOff>123357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC51C516-5628-4805-9AA5-36B357FDA326}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="67056000"/>
+          <a:ext cx="9314286" cy="3742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>373</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>151238</xdr:colOff>
+      <xdr:row>391</xdr:row>
+      <xdr:rowOff>37667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56350AC-77C5-4CFC-B2C1-087BF917CE5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="71056500"/>
+          <a:ext cx="9295238" cy="3466667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -602,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
@@ -632,4 +1319,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAAC251-ED6D-4BF5-BCA9-1565F0D72D3D}">
+  <dimension ref="A2:B373"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="B374" sqref="B374"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>